<commit_message>
created graphs some lit
finish lit review
</commit_message>
<xml_diff>
--- a/questionnaire results.xlsx
+++ b/questionnaire results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adam\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adam\Documents\GitHub\Dissertation-educational_robots\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t>question</t>
   </si>
@@ -94,8 +94,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,10 +403,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,9 +414,11 @@
     <col min="1" max="1" width="46" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="46" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -434,8 +437,26 @@
       <c r="F1" t="s">
         <v>10</v>
       </c>
+      <c r="H1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -445,8 +466,44 @@
       <c r="C2">
         <v>9</v>
       </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1">
+        <f>B2/N2</f>
+        <v>0.1</v>
+      </c>
+      <c r="J2" s="1">
+        <f>C2/N2</f>
+        <v>0.9</v>
+      </c>
+      <c r="K2" s="1">
+        <f>D2/N2</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <f>E2/N2</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="1">
+        <f>F2/N2</f>
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <f>SUM(B2:F2)</f>
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -459,8 +516,41 @@
       <c r="D3">
         <v>2</v>
       </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" ref="I3:I6" si="0">B3/N3</f>
+        <v>0.3</v>
+      </c>
+      <c r="J3" s="1">
+        <f t="shared" ref="J3:J6" si="1">C3/N3</f>
+        <v>0.5</v>
+      </c>
+      <c r="K3" s="1">
+        <f t="shared" ref="K3:K6" si="2">D3/N3</f>
+        <v>0.2</v>
+      </c>
+      <c r="L3" s="1">
+        <f t="shared" ref="L3:L6" si="3">E3/N3</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="1">
+        <f t="shared" ref="M3:M6" si="4">F3/N3</f>
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N6" si="5">SUM(B3:F3)</f>
+        <v>10</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -476,8 +566,35 @@
       <c r="F4">
         <v>1</v>
       </c>
+      <c r="H4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="K4" s="1">
+        <f t="shared" si="2"/>
+        <v>0.3</v>
+      </c>
+      <c r="L4" s="1">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="M4" s="1">
+        <f t="shared" si="4"/>
+        <v>0.1</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -490,8 +607,41 @@
       <c r="D5">
         <v>2</v>
       </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="1"/>
+        <v>0.3</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="L5" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -500,9 +650,46 @@
       </c>
       <c r="C6">
         <v>5</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="1"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="K6" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M6" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="5"/>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>